<commit_message>
refactoring to a function
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsrizki/Downloads/BACKEND-V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A3498-89FC-D54A-8E3C-E0F6CAEB5CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CB12A4-ACAD-8746-8C4D-D7D8DE6A289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="21900" xr2:uid="{3A87F806-BAD1-421D-90D2-A181B0C5DCFA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{3A87F806-BAD1-421D-90D2-A181B0C5DCFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1221,7 +1221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1282,6 +1282,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1600,14 +1606,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797D938F-3F45-4CD5-BE51-20AEFDF10127}">
   <dimension ref="B1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="38.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" style="2" customWidth="1"/>
     <col min="6" max="8" width="9.1640625" style="2"/>
@@ -1705,8 +1711,8 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="2:9" ht="96" x14ac:dyDescent="0.2">
-      <c r="C13" s="13" t="s">
+    <row r="13" spans="2:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C13" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2079,8 +2085,8 @@
       </c>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="3:9" ht="96" x14ac:dyDescent="0.2">
-      <c r="C36" s="18" t="s">
+    <row r="36" spans="3:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C36" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2201,8 +2207,8 @@
       </c>
       <c r="I41" s="14"/>
     </row>
-    <row r="42" spans="3:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="C42" s="18" t="s">
+    <row r="42" spans="3:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C42" s="26" t="s">
         <v>34</v>
       </c>
       <c r="D42" s="3" t="s">

</xml_diff>